<commit_message>
Updating new tests added and adjustments to new folder structure
</commit_message>
<xml_diff>
--- a/nep-automation/src/main/java/DataFiles/DataFile.xlsx
+++ b/nep-automation/src/main/java/DataFiles/DataFile.xlsx
@@ -1,27 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Intellij\15\NetayaSWG\Automation\src\test\java\DataFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Intellij\18\NetayaSWG\Automation\src\main\java\DataFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85F83CDF-65DF-414E-9780-115AED14FA70}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A5AC9E8-8333-40C1-BC22-34295013A6F7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{0813270D-BFFB-4065-B4A0-DD50BA55F9DE}"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="13176" firstSheet="2" activeTab="5" xr2:uid="{0813270D-BFFB-4065-B4A0-DD50BA55F9DE}"/>
   </bookViews>
   <sheets>
-    <sheet name="SAMLTest" sheetId="15" r:id="rId1"/>
-    <sheet name="InstallEndPoint" sheetId="14" r:id="rId2"/>
-    <sheet name="DownloadFromPortal" sheetId="13" r:id="rId3"/>
-    <sheet name="InstallApplication" sheetId="6" r:id="rId4"/>
-    <sheet name="BlockURLTest" sheetId="8" r:id="rId5"/>
-    <sheet name="BlockEicarTest" sheetId="11" r:id="rId6"/>
-    <sheet name="BlockEicarEnterprise" sheetId="12" r:id="rId7"/>
-    <sheet name="PolicyTest" sheetId="9" r:id="rId8"/>
-    <sheet name="PolicyTestProd" sheetId="10" r:id="rId9"/>
+    <sheet name="InstallApplication" sheetId="6" r:id="rId1"/>
+    <sheet name="SAMLTest" sheetId="15" r:id="rId2"/>
+    <sheet name="DownloadFromPortalTest" sheetId="13" r:id="rId3"/>
+    <sheet name="InstallEndPointTest" sheetId="14" r:id="rId4"/>
+    <sheet name="VerifyEndPointOkAtPortalTest" sheetId="16" r:id="rId5"/>
+    <sheet name="ClientLogToPortalTest" sheetId="18" r:id="rId6"/>
+    <sheet name="BlockURLTest" sheetId="8" r:id="rId7"/>
+    <sheet name="BlockEicarTest" sheetId="11" r:id="rId8"/>
+    <sheet name="BlockEicarEnterprise" sheetId="12" r:id="rId9"/>
+    <sheet name="PolicyTest" sheetId="9" r:id="rId10"/>
+    <sheet name="PolicyTestProd" sheetId="10" r:id="rId11"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="102">
   <si>
     <t>Description</t>
   </si>
@@ -206,21 +208,12 @@
     <t>Customer</t>
   </si>
   <si>
-    <t>NepAutomationCustomer</t>
-  </si>
-  <si>
     <t>Wait files to be downloaded timeout in seconds</t>
   </si>
   <si>
     <t>120</t>
   </si>
   <si>
-    <t>client.pem, client_key.pem, TrustwaveEndpoint.exe</t>
-  </si>
-  <si>
-    <t>Expected Files</t>
-  </si>
-  <si>
     <t>Service Start/Stop timeout</t>
   </si>
   <si>
@@ -297,6 +290,63 @@
   </si>
   <si>
     <t>Trustwave123</t>
+  </si>
+  <si>
+    <t>Wait for publish to be completed</t>
+  </si>
+  <si>
+    <t>Wait because File is still being processed (virus scanned and stored)</t>
+  </si>
+  <si>
+    <t>Report Interval</t>
+  </si>
+  <si>
+    <t>Event Type</t>
+  </si>
+  <si>
+    <t>INFORMATION</t>
+  </si>
+  <si>
+    <t>Event ID</t>
+  </si>
+  <si>
+    <t>Event Log</t>
+  </si>
+  <si>
+    <t>APPLICATION</t>
+  </si>
+  <si>
+    <t>Event Source</t>
+  </si>
+  <si>
+    <t>AutomationTest</t>
+  </si>
+  <si>
+    <t>Hello!! this is the test info</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>Event Description</t>
+  </si>
+  <si>
+    <t>Add time stamp to description</t>
+  </si>
+  <si>
+    <t>123</t>
+  </si>
+  <si>
+    <t>Log To Appear Timeout</t>
+  </si>
+  <si>
+    <t>300</t>
+  </si>
+  <si>
+    <t>TrustwaveEP Automation #3</t>
+  </si>
+  <si>
+    <t>180</t>
   </si>
 </sst>
 </file>
@@ -682,10 +732,337 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBC9FAC2-0100-466A-9965-E590FD28E573}">
+  <sheetPr codeName="Sheet5"/>
+  <dimension ref="A1:O2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="11.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="34.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="60.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="23.21875" style="1" customWidth="1"/>
+    <col min="14" max="14" width="19.77734375" style="1" customWidth="1"/>
+    <col min="15" max="16384" width="8.77734375" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="M2" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="L2" r:id="rId1" xr:uid="{775B0F99-60BA-4F30-ADF4-E438A52E96BB}"/>
+    <hyperlink ref="M2" r:id="rId2" xr:uid="{B0FE7253-12EF-420F-B1B6-87A3909B8136}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FED038C0-817F-472E-AD39-DAEB143C92CB}">
+  <dimension ref="A1:K2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="59.21875" customWidth="1"/>
+    <col min="3" max="3" width="55" customWidth="1"/>
+    <col min="4" max="4" width="47" customWidth="1"/>
+    <col min="5" max="5" width="42.5546875" customWidth="1"/>
+    <col min="6" max="6" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="30.77734375" customWidth="1"/>
+    <col min="8" max="8" width="29.109375" customWidth="1"/>
+    <col min="9" max="9" width="35.21875" customWidth="1"/>
+    <col min="10" max="10" width="26.77734375" customWidth="1"/>
+    <col min="11" max="11" width="30.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" t="s">
+        <v>37</v>
+      </c>
+      <c r="H1" t="s">
+        <v>38</v>
+      </c>
+      <c r="I1" t="s">
+        <v>41</v>
+      </c>
+      <c r="J1" t="s">
+        <v>42</v>
+      </c>
+      <c r="K1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" t="s">
+        <v>36</v>
+      </c>
+      <c r="F2" t="s">
+        <v>35</v>
+      </c>
+      <c r="G2" t="s">
+        <v>46</v>
+      </c>
+      <c r="H2" t="s">
+        <v>39</v>
+      </c>
+      <c r="I2" t="s">
+        <v>44</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="K2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="J2" r:id="rId1" xr:uid="{61D87B81-55A6-4A85-A612-C5F1FF928734}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3590BECC-6F16-49AF-A187-EF8E4637F50A}">
+  <dimension ref="A1:K2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="59.21875" customWidth="1"/>
+    <col min="3" max="3" width="55" customWidth="1"/>
+    <col min="4" max="4" width="47" customWidth="1"/>
+    <col min="5" max="5" width="42.5546875" customWidth="1"/>
+    <col min="6" max="6" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="30.77734375" customWidth="1"/>
+    <col min="8" max="8" width="29.109375" customWidth="1"/>
+    <col min="9" max="9" width="35.21875" customWidth="1"/>
+    <col min="10" max="10" width="26.77734375" customWidth="1"/>
+    <col min="11" max="11" width="30.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" t="s">
+        <v>37</v>
+      </c>
+      <c r="H1" t="s">
+        <v>38</v>
+      </c>
+      <c r="I1" t="s">
+        <v>41</v>
+      </c>
+      <c r="J1" t="s">
+        <v>42</v>
+      </c>
+      <c r="K1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" t="s">
+        <v>36</v>
+      </c>
+      <c r="F2" t="s">
+        <v>35</v>
+      </c>
+      <c r="G2" t="s">
+        <v>46</v>
+      </c>
+      <c r="H2" t="s">
+        <v>39</v>
+      </c>
+      <c r="I2" t="s">
+        <v>44</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="K2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="J2" r:id="rId1" xr:uid="{8C3F443D-9EA8-4324-BCF3-ABB98314F668}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{370C0B2F-291F-41F7-BBEC-60B7B7B7C290}">
   <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
@@ -693,14 +1070,14 @@
   <cols>
     <col min="1" max="1" width="24.5546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="27.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.77734375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
     <col min="5" max="8" width="23.77734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -709,33 +1086,33 @@
         <v>6</v>
       </c>
       <c r="D1" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="E1" t="s">
+        <v>65</v>
+      </c>
+      <c r="F1" t="s">
+        <v>66</v>
+      </c>
+      <c r="G1" t="s">
+        <v>67</v>
+      </c>
+      <c r="H1" t="s">
         <v>68</v>
-      </c>
-      <c r="F1" t="s">
-        <v>69</v>
-      </c>
-      <c r="G1" t="s">
-        <v>70</v>
-      </c>
-      <c r="H1" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B2" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C2" t="s">
         <v>7</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>23</v>
@@ -744,7 +1121,7 @@
         <v>23</v>
       </c>
       <c r="G2" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="H2" t="s">
         <v>25</v>
@@ -752,25 +1129,25 @@
     </row>
     <row r="3" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B3" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C3" t="s">
         <v>7</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>23</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>25</v>
@@ -778,25 +1155,25 @@
     </row>
     <row r="4" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B4" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C4" t="s">
         <v>7</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>23</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="H4" s="1" t="s">
         <v>25</v>
@@ -804,51 +1181,51 @@
     </row>
     <row r="5" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B5" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C5" t="s">
         <v>7</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B6" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C6" t="s">
         <v>7</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>23</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="H6" s="1" t="s">
         <v>25</v>
@@ -867,71 +1244,25 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28112D5D-4D41-49B5-9C1F-91FA6EFF3BC2}">
-  <dimension ref="A1:D2"/>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC204677-932F-42E3-A329-F307B9A37F9B}">
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="34.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="42.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="31.77734375" customWidth="1"/>
+    <col min="5" max="5" width="56.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="40.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="40.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>63</v>
-      </c>
-      <c r="B1" t="s">
-        <v>62</v>
-      </c>
-      <c r="C1" t="s">
-        <v>61</v>
-      </c>
-      <c r="D1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC204677-932F-42E3-A329-F307B9A37F9B}">
-  <dimension ref="A1:E2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="2" max="2" width="22.21875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="31.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="47.77734375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -939,31 +1270,39 @@
         <v>54</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="E1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+        <v>83</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="G1" s="1"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>55</v>
+        <v>100</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="E2" t="s">
-        <v>58</v>
-      </c>
+        <v>56</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G2" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -972,131 +1311,177 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBC9FAC2-0100-466A-9965-E590FD28E573}">
-  <sheetPr codeName="Sheet5"/>
-  <dimension ref="A1:O2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28112D5D-4D41-49B5-9C1F-91FA6EFF3BC2}">
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="22.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="34.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="60.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="23.33203125" style="1" customWidth="1"/>
-    <col min="14" max="14" width="19.88671875" style="1" customWidth="1"/>
-    <col min="15" max="16384" width="8.6640625" style="1"/>
+    <col min="1" max="2" width="34.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="42.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>23</v>
+        <v>101</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>24</v>
+        <v>101</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>25</v>
+        <v>101</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="L2" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="M2" s="4" t="s">
-        <v>33</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="L2" r:id="rId1" xr:uid="{775B0F99-60BA-4F30-ADF4-E438A52E96BB}"/>
-    <hyperlink ref="M2" r:id="rId2" xr:uid="{B0FE7253-12EF-420F-B1B6-87A3909B8136}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFC2CA0F-1477-46C2-9AA1-8A5670F4E730}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I31" sqref="I31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="24.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77C3FA84-DBAF-4AD9-B8F6-55B860096D54}">
+  <dimension ref="A1:J2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="34.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="8" width="34.21875" customWidth="1"/>
+    <col min="9" max="9" width="42.5546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="42.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D1" t="s">
+        <v>98</v>
+      </c>
+      <c r="E1" t="s">
+        <v>86</v>
+      </c>
+      <c r="F1" t="s">
+        <v>88</v>
+      </c>
+      <c r="G1" t="s">
+        <v>89</v>
+      </c>
+      <c r="H1" t="s">
+        <v>91</v>
+      </c>
+      <c r="I1" t="s">
+        <v>95</v>
+      </c>
+      <c r="J1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C21916EB-A6DC-450A-A85F-A34B0CFEF38D}">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -1106,8 +1491,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.77734375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19.109375" customWidth="1"/>
     <col min="4" max="4" width="54" customWidth="1"/>
   </cols>
@@ -1137,7 +1522,7 @@
         <v>5</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>
@@ -1149,7 +1534,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38C4480A-E140-45C4-BF8D-587C885F562F}">
   <dimension ref="A1:D4"/>
   <sheetViews>
@@ -1159,8 +1544,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.77734375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19.109375" customWidth="1"/>
     <col min="4" max="4" width="62.44140625" bestFit="1" customWidth="1"/>
   </cols>
@@ -1231,7 +1616,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B53D489-3AD9-4691-BEB7-D49122815826}">
   <dimension ref="A1:D4"/>
   <sheetViews>
@@ -1241,10 +1626,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.77734375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19.109375" customWidth="1"/>
-    <col min="4" max="4" width="67.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="67.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
@@ -1309,206 +1694,4 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FED038C0-817F-472E-AD39-DAEB143C92CB}">
-  <dimension ref="A1:K2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="2" max="2" width="59.33203125" customWidth="1"/>
-    <col min="3" max="3" width="55" customWidth="1"/>
-    <col min="4" max="4" width="47" customWidth="1"/>
-    <col min="5" max="5" width="42.5546875" customWidth="1"/>
-    <col min="6" max="6" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="30.6640625" customWidth="1"/>
-    <col min="8" max="8" width="29.109375" customWidth="1"/>
-    <col min="9" max="9" width="35.33203125" customWidth="1"/>
-    <col min="10" max="10" width="26.88671875" customWidth="1"/>
-    <col min="11" max="11" width="30.109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1" t="s">
-        <v>40</v>
-      </c>
-      <c r="C1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F1" t="s">
-        <v>2</v>
-      </c>
-      <c r="G1" t="s">
-        <v>37</v>
-      </c>
-      <c r="H1" t="s">
-        <v>38</v>
-      </c>
-      <c r="I1" t="s">
-        <v>41</v>
-      </c>
-      <c r="J1" t="s">
-        <v>42</v>
-      </c>
-      <c r="K1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="C2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" t="s">
-        <v>36</v>
-      </c>
-      <c r="F2" t="s">
-        <v>35</v>
-      </c>
-      <c r="G2" t="s">
-        <v>46</v>
-      </c>
-      <c r="H2" t="s">
-        <v>39</v>
-      </c>
-      <c r="I2" t="s">
-        <v>44</v>
-      </c>
-      <c r="J2" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="K2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="J2" r:id="rId1" xr:uid="{61D87B81-55A6-4A85-A612-C5F1FF928734}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3590BECC-6F16-49AF-A187-EF8E4637F50A}">
-  <dimension ref="A1:K2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="2" max="2" width="59.33203125" customWidth="1"/>
-    <col min="3" max="3" width="55" customWidth="1"/>
-    <col min="4" max="4" width="47" customWidth="1"/>
-    <col min="5" max="5" width="42.5546875" customWidth="1"/>
-    <col min="6" max="6" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="30.6640625" customWidth="1"/>
-    <col min="8" max="8" width="29.109375" customWidth="1"/>
-    <col min="9" max="9" width="35.33203125" customWidth="1"/>
-    <col min="10" max="10" width="26.88671875" customWidth="1"/>
-    <col min="11" max="11" width="30.109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1" t="s">
-        <v>40</v>
-      </c>
-      <c r="C1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F1" t="s">
-        <v>2</v>
-      </c>
-      <c r="G1" t="s">
-        <v>37</v>
-      </c>
-      <c r="H1" t="s">
-        <v>38</v>
-      </c>
-      <c r="I1" t="s">
-        <v>41</v>
-      </c>
-      <c r="J1" t="s">
-        <v>42</v>
-      </c>
-      <c r="K1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="C2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" t="s">
-        <v>36</v>
-      </c>
-      <c r="F2" t="s">
-        <v>35</v>
-      </c>
-      <c r="G2" t="s">
-        <v>46</v>
-      </c>
-      <c r="H2" t="s">
-        <v>39</v>
-      </c>
-      <c r="I2" t="s">
-        <v>44</v>
-      </c>
-      <c r="J2" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="K2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="J2" r:id="rId1" xr:uid="{8C3F443D-9EA8-4324-BCF3-ABB98314F668}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
-</worksheet>
 </file>
</xml_diff>